<commit_message>
Added SOLE batch notebook; updated docker/makefile to support dynamic port at runtime
</commit_message>
<xml_diff>
--- a/beta_bruteforce_3x3_99x99.xlsx
+++ b/beta_bruteforce_3x3_99x99.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\arc\research\projects\supy-res-imaging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9053172-93C3-47C4-A1EA-B7BA2C3295B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8A673A-7503-4842-B160-EDBF267343AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -279,6 +279,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +597,8 @@
   <dimension ref="A1:BA43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BA10" activeCellId="10" sqref="AQ11 AR10 AS10 AT11 AU11 AV11 AW11 AX11 AY11 AZ10 BA10"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1800,7 @@
       <c r="AE8" s="5">
         <v>1.115962745</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AF8" s="6">
         <v>1.1084197149999999</v>
       </c>
       <c r="AG8">
@@ -2589,7 +2590,7 @@
       <c r="AE13">
         <v>1.1261937529999999</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="5">
         <v>1.102144164</v>
       </c>
       <c r="AG13" s="5">

</xml_diff>

<commit_message>
Included notebook on laplacian of gaussian filter
</commit_message>
<xml_diff>
--- a/beta_bruteforce_3x3_99x99.xlsx
+++ b/beta_bruteforce_3x3_99x99.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\arc\research\projects\supy-res-imaging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arc\AppData\Local\Temp\scp00215\home\arc\Desktop\supy-res-imaging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8A673A-7503-4842-B160-EDBF267343AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06479CA6-8DAA-4951-A809-0BC974FD314A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>